<commit_message>
up 2019-11-11 9:44 xu
up
</commit_message>
<xml_diff>
--- a/沈阳鹏斓面辅料采购程序/表2.尺码搭配表.xlsx
+++ b/沈阳鹏斓面辅料采购程序/表2.尺码搭配表.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zhu\Business\面辅料采购程序\新建文件夹\新建文件夹\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB21520-5B4F-412C-B3F8-E3A743E4C8B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CFF77DA2-076E-408D-837D-275C64FF7027}"/>
+    <workbookView windowWidth="17880" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="RGL1" sheetId="1" r:id="rId1"/>
@@ -20,17 +14,12 @@
     <sheet name="D.PANT" sheetId="5" r:id="rId5"/>
     <sheet name="C.PANT" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="93">
   <si>
     <t>LOT#</t>
   </si>
@@ -42,14 +31,18 @@
   </si>
   <si>
     <t>COLOR</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>COLOR#</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Dotum"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">JACKET </t>
     </r>
     <r>
@@ -58,7 +51,6 @@
         <sz val="9"/>
         <color indexed="8"/>
         <rFont val="Dotum"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>上衣</t>
@@ -66,147 +58,111 @@
   </si>
   <si>
     <t>34R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>36R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>38R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>40R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>42R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>44R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>46R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>48R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>50R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>52R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>54R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>56R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>58R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>60R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>62R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>36L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>38L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>40L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>42L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>44L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>46L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>48L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>50L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>52L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>54L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>56L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>58L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>60L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>62L</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>34S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>36S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>38S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>40S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>42S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>44S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>46S</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Sub Total: </t>
@@ -222,6 +178,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>颜</t>
     </r>
     <r>
@@ -230,15 +193,20 @@
         <sz val="9"/>
         <color indexed="8"/>
         <rFont val="Dotum"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>色</t>
     </r>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>颜</t>
     </r>
     <r>
@@ -247,15 +215,19 @@
         <sz val="9"/>
         <color indexed="8"/>
         <rFont val="Dotum"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>色编号</t>
     </r>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Dotum"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">PANT </t>
     </r>
     <r>
@@ -264,7 +236,6 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>裤</t>
@@ -275,7 +246,6 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Dotum"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>子</t>
@@ -283,6 +253,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>订单</t>
     </r>
     <r>
@@ -291,7 +268,6 @@
         <sz val="9"/>
         <color indexed="8"/>
         <rFont val="Dotum"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>合</t>
@@ -302,71 +278,182 @@
         <sz val="9"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>计</t>
     </r>
   </si>
+  <si>
+    <t>TEXTMIAN</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>text3</t>
+  </si>
+  <si>
+    <t>text4</t>
+  </si>
+  <si>
+    <t>text5</t>
+  </si>
+  <si>
+    <t>text6</t>
+  </si>
+  <si>
+    <t>text7</t>
+  </si>
+  <si>
+    <t>text8</t>
+  </si>
+  <si>
+    <t>text9</t>
+  </si>
+  <si>
+    <t>text10</t>
+  </si>
+  <si>
+    <t>text11</t>
+  </si>
+  <si>
+    <t>text12</t>
+  </si>
+  <si>
+    <t>text13</t>
+  </si>
+  <si>
+    <t>text14</t>
+  </si>
+  <si>
+    <t>text15</t>
+  </si>
+  <si>
+    <t>text16</t>
+  </si>
+  <si>
+    <t>text17</t>
+  </si>
+  <si>
+    <t>text18</t>
+  </si>
+  <si>
+    <t>text19</t>
+  </si>
+  <si>
+    <t>text20</t>
+  </si>
+  <si>
+    <t>text21</t>
+  </si>
+  <si>
+    <t>text22</t>
+  </si>
+  <si>
+    <t>text23</t>
+  </si>
+  <si>
+    <t>text24</t>
+  </si>
+  <si>
+    <t>text25</t>
+  </si>
+  <si>
+    <t>text26</t>
+  </si>
+  <si>
+    <t>text27</t>
+  </si>
+  <si>
+    <t>text28</t>
+  </si>
+  <si>
+    <t>text29</t>
+  </si>
+  <si>
+    <t>text30</t>
+  </si>
+  <si>
+    <t>text31</t>
+  </si>
+  <si>
+    <t>text32</t>
+  </si>
+  <si>
+    <t>text33</t>
+  </si>
+  <si>
+    <t>text34</t>
+  </si>
+  <si>
+    <t>text35</t>
+  </si>
+  <si>
+    <t>text36</t>
+  </si>
+  <si>
+    <t>text37</t>
+  </si>
+  <si>
+    <t>text38</t>
+  </si>
+  <si>
+    <t>text39</t>
+  </si>
+  <si>
+    <t>text40</t>
+  </si>
+  <si>
+    <t>text41</t>
+  </si>
+  <si>
+    <t>text42</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Dotum"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color indexed="8"/>
       <name val="Dotum"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <color indexed="8"/>
+      <name val="Dotum"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Dotum"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Dotum"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -374,7 +461,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Dotum"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -382,7 +468,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -390,11 +475,159 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,12 +636,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -418,162 +831,307 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,10 +1139,10 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,299 +1150,440 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1" xr:uid="{5830E15B-05BD-4B5C-A47F-F9E691ABD933}"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规 2" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -933,7 +1632,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -966,26 +1665,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1018,23 +1700,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1176,24 +1841,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33182F02-915D-472E-A624-3804275A7A8B}">
-  <dimension ref="A1:AQ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="3" max="3" width="8.125" customWidth="1"/>
@@ -1201,767 +1861,901 @@
     <col min="7" max="42" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" ht="22.5" spans="1:43">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="22" t="s">
+      <c r="AI1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="22" t="s">
+      <c r="AP1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AQ1" s="36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" ht="24.75" spans="1:43">
+      <c r="A2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="29">
         <v>28</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="30">
         <v>30</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="30">
         <v>32</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="30">
         <v>34</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="30">
         <v>36</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="30">
         <v>38</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="30">
         <v>40</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="30">
         <v>42</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="30">
         <v>44</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="30">
         <v>46</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="30">
         <v>48</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="30">
         <v>50</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="30">
         <v>52</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="30">
         <v>54</v>
       </c>
-      <c r="U2" s="23">
+      <c r="U2" s="32">
         <v>56</v>
       </c>
-      <c r="V2" s="24">
+      <c r="V2" s="33">
         <v>30</v>
       </c>
-      <c r="W2" s="10">
+      <c r="W2" s="30">
         <v>32</v>
       </c>
-      <c r="X2" s="10">
+      <c r="X2" s="30">
         <v>34</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="Y2" s="30">
         <v>36</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="Z2" s="30">
         <v>38</v>
       </c>
-      <c r="AA2" s="10">
+      <c r="AA2" s="30">
         <v>40</v>
       </c>
-      <c r="AB2" s="10">
+      <c r="AB2" s="30">
         <v>42</v>
       </c>
-      <c r="AC2" s="10">
+      <c r="AC2" s="30">
         <v>44</v>
       </c>
-      <c r="AD2" s="10">
+      <c r="AD2" s="30">
         <v>46</v>
       </c>
-      <c r="AE2" s="10">
+      <c r="AE2" s="30">
         <v>48</v>
       </c>
-      <c r="AF2" s="10">
+      <c r="AF2" s="30">
         <v>50</v>
       </c>
-      <c r="AG2" s="10">
+      <c r="AG2" s="30">
         <v>52</v>
       </c>
-      <c r="AH2" s="10">
+      <c r="AH2" s="30">
         <v>54</v>
       </c>
-      <c r="AI2" s="23">
+      <c r="AI2" s="32">
         <v>56</v>
       </c>
-      <c r="AJ2" s="24">
+      <c r="AJ2" s="33">
         <v>28</v>
       </c>
-      <c r="AK2" s="10">
+      <c r="AK2" s="30">
         <v>30</v>
       </c>
-      <c r="AL2" s="10">
+      <c r="AL2" s="30">
         <v>32</v>
       </c>
-      <c r="AM2" s="10">
+      <c r="AM2" s="30">
         <v>34</v>
       </c>
-      <c r="AN2" s="10">
+      <c r="AN2" s="30">
         <v>36</v>
       </c>
-      <c r="AO2" s="10">
+      <c r="AO2" s="30">
         <v>38</v>
       </c>
-      <c r="AP2" s="23">
+      <c r="AP2" s="32">
         <v>40</v>
       </c>
-      <c r="AQ2" s="26" t="s">
+      <c r="AQ2" s="37" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91B9F6D-5386-4BF5-96E7-7F8A3355B9A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="7" max="42" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" ht="22.5" spans="1:43">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="22" t="s">
+      <c r="AI1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="21" t="s">
+      <c r="AJ1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="22" t="s">
+      <c r="AP1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AQ1" s="36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" ht="24.75" spans="1:43">
+      <c r="A2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="29">
         <v>28</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="30">
         <v>30</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="30">
         <v>32</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="30">
         <v>34</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="30">
         <v>36</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="30">
         <v>38</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="30">
         <v>40</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="30">
         <v>42</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="30">
         <v>44</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="30">
         <v>46</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="30">
         <v>48</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="30">
         <v>50</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="30">
         <v>52</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="30">
         <v>54</v>
       </c>
-      <c r="U2" s="23">
+      <c r="U2" s="32">
         <v>56</v>
       </c>
-      <c r="V2" s="24">
+      <c r="V2" s="33">
         <v>30</v>
       </c>
-      <c r="W2" s="10">
+      <c r="W2" s="30">
         <v>32</v>
       </c>
-      <c r="X2" s="10">
+      <c r="X2" s="30">
         <v>34</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="Y2" s="30">
         <v>36</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="Z2" s="30">
         <v>38</v>
       </c>
-      <c r="AA2" s="10">
+      <c r="AA2" s="30">
         <v>40</v>
       </c>
-      <c r="AB2" s="10">
+      <c r="AB2" s="30">
         <v>42</v>
       </c>
-      <c r="AC2" s="10">
+      <c r="AC2" s="30">
         <v>44</v>
       </c>
-      <c r="AD2" s="10">
+      <c r="AD2" s="30">
         <v>46</v>
       </c>
-      <c r="AE2" s="10">
+      <c r="AE2" s="30">
         <v>48</v>
       </c>
-      <c r="AF2" s="10">
+      <c r="AF2" s="30">
         <v>50</v>
       </c>
-      <c r="AG2" s="10">
+      <c r="AG2" s="30">
         <v>52</v>
       </c>
-      <c r="AH2" s="10">
+      <c r="AH2" s="30">
         <v>54</v>
       </c>
-      <c r="AI2" s="23">
+      <c r="AI2" s="32">
         <v>56</v>
       </c>
-      <c r="AJ2" s="24">
+      <c r="AJ2" s="33">
         <v>28</v>
       </c>
-      <c r="AK2" s="10">
+      <c r="AK2" s="30">
         <v>30</v>
       </c>
-      <c r="AL2" s="10">
+      <c r="AL2" s="30">
         <v>32</v>
       </c>
-      <c r="AM2" s="10">
+      <c r="AM2" s="30">
         <v>34</v>
       </c>
-      <c r="AN2" s="10">
+      <c r="AN2" s="30">
         <v>36</v>
       </c>
-      <c r="AO2" s="10">
+      <c r="AO2" s="30">
         <v>38</v>
       </c>
-      <c r="AP2" s="23">
+      <c r="AP2" s="32">
         <v>40</v>
       </c>
-      <c r="AQ2" s="26" t="s">
+      <c r="AQ2" s="37" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F106C45-7338-43B6-8389-95EE4BA268A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AC2"/>
+      <selection activeCell="A1" sqref="A1:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="7" max="28" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" ht="22.5" spans="1:29">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" ht="24.75" spans="1:29">
+      <c r="A2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="29">
         <v>28</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="30">
         <v>30</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="30">
         <v>32</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="30">
         <v>34</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="30">
         <v>36</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="30">
         <v>38</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="30">
         <v>40</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="32">
         <v>42</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="33">
         <v>30</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="30">
         <v>32</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="30">
         <v>34</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="30">
         <v>36</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="30">
         <v>38</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="30">
         <v>40</v>
       </c>
-      <c r="U2" s="23">
+      <c r="U2" s="32">
         <v>42</v>
       </c>
-      <c r="V2" s="24">
+      <c r="V2" s="33">
         <v>28</v>
       </c>
-      <c r="W2" s="10">
+      <c r="W2" s="30">
         <v>30</v>
       </c>
-      <c r="X2" s="10">
+      <c r="X2" s="30">
         <v>32</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="Y2" s="30">
         <v>34</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="Z2" s="30">
         <v>36</v>
       </c>
-      <c r="AA2" s="10">
+      <c r="AA2" s="30">
         <v>38</v>
       </c>
-      <c r="AB2" s="10">
+      <c r="AB2" s="30">
         <v>40</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AC2" s="35" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586F44A5-97AF-4C2F-A90B-882594636B76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="7" max="42" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" ht="19.5" customHeight="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1974,178 +2768,178 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="X1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="35" t="s">
+      <c r="Y1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="35" t="s">
+      <c r="Z1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="35" t="s">
+      <c r="AA1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="35" t="s">
+      <c r="AC1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="35" t="s">
+      <c r="AD1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="35" t="s">
+      <c r="AE1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="35" t="s">
+      <c r="AF1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="35" t="s">
+      <c r="AG1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="35" t="s">
+      <c r="AH1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="36" t="s">
+      <c r="AI1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="34" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="35" t="s">
+      <c r="AK1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="35" t="s">
+      <c r="AL1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="35" t="s">
+      <c r="AM1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="35" t="s">
+      <c r="AN1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="35" t="s">
+      <c r="AO1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="36" t="s">
+      <c r="AP1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="29" t="s">
+      <c r="AQ1" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="14.25" spans="1:43">
+      <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="31"/>
-      <c r="AL2" s="31"/>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="37" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="19" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2153,37 +2947,39 @@
   <mergeCells count="1">
     <mergeCell ref="F1:F2"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCEA73E-1C08-492A-BECC-057507F99605}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86069AA-6F78-4D69-8879-354C266FC09A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
up yao 2019-12-27 13：37
update yao
</commit_message>
<xml_diff>
--- a/沈阳鹏斓面辅料采购程序/表2.尺码搭配表.xlsx
+++ b/沈阳鹏斓面辅料采购程序/表2.尺码搭配表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7860" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RGL1" sheetId="1" r:id="rId1"/>
@@ -805,9 +805,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="46">
@@ -944,25 +944,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -975,7 +960,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -990,64 +997,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1068,9 +1017,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1090,6 +1085,11 @@
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1148,25 +1148,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1190,7 +1178,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1202,7 +1238,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,67 +1310,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1290,48 +1332,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="48">
     <border>
@@ -1859,6 +1859,17 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1874,6 +1885,54 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1896,65 +1955,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -1968,10 +1968,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1980,136 +1980,136 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="43" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="45" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="3" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -2770,13 +2770,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="3" max="3" width="8.125" customWidth="1"/>
@@ -3044,6 +3044,29 @@
       </c>
       <c r="AQ2" s="103" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="7:13">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3058,8 +3081,8 @@
   <sheetPr/>
   <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
@@ -3198,7 +3221,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" ht="15" spans="1:43">
+    <row r="2" spans="1:43">
       <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
@@ -3329,49 +3352,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:43">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="79"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="79"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="78"/>
-      <c r="AQ3" s="104"/>
+    <row r="3" spans="7:12">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3382,13 +3381,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A$1:F$1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
     <col min="7" max="28" width="3.625" customWidth="1"/>
   </cols>
@@ -3569,6 +3568,17 @@
       </c>
       <c r="AC2" s="91" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="7:9">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3580,13 +3590,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
     <col min="7" max="42" width="3.625" customWidth="1"/>
   </cols>
@@ -3779,6 +3789,17 @@
         <v>51</v>
       </c>
     </row>
+    <row r="3" spans="7:9">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:F2"/>
@@ -3792,13 +3813,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:AP4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="6" width="7.125" customWidth="1"/>
     <col min="7" max="41" width="3.625" customWidth="1"/>
@@ -4124,6 +4145,17 @@
       </c>
       <c r="AP3" s="110" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="7:9">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4148,13 +4180,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AG19" sqref="AG19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
     <col min="7" max="41" width="3.625" customWidth="1"/>
   </cols>
@@ -4363,6 +4395,17 @@
       </c>
       <c r="AP2" s="113" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="7:9">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4389,7 +4432,7 @@
   <dimension ref="A1:AQ23"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>